<commit_message>
fuel_price and fuel_price_change_annual logging: which profile is simulated theoretical, not implemented constraint for off-grid operation - not needed as genset=peakdemand
</commit_message>
<xml_diff>
--- a/inputs/reliable_no_mgs.xlsx
+++ b/inputs/reliable_no_mgs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -3426,7 +3426,7 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -3871,8 +3871,8 @@
   </sheetPr>
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4393,7 +4393,7 @@
         <v>144</v>
       </c>
       <c r="B47" s="18" t="n">
-        <v>0.63</v>
+        <v>0.68</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>145</v>
@@ -30838,8 +30838,8 @@
   </sheetPr>
   <dimension ref="A1:AMG36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -46285,16 +46285,16 @@
         <v>43</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F17" s="39" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G17" s="39" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H17" s="39" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
nearing calculation for main grid extension costs
</commit_message>
<xml_diff>
--- a/inputs/reliable_no_mgs.xlsx
+++ b/inputs/reliable_no_mgs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3447" uniqueCount="934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3447" uniqueCount="933">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -2805,7 +2805,7 @@
     <t xml:space="preserve">number_of_equal_generators</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
+    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">capacity_pcc_consumption_kW</t>
@@ -2815,9 +2815,6 @@
   </si>
   <si>
     <t xml:space="preserve">default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">share_hybrid</t>
@@ -3145,12 +3142,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3432,8 +3429,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3592,7 +3589,7 @@
         <v>44</v>
       </c>
       <c r="C17" s="18" t="n">
-        <v>7</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3877,8 +3874,8 @@
   </sheetPr>
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4286,7 +4283,7 @@
         <v>134</v>
       </c>
       <c r="B37" s="18" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>113</v>
@@ -4597,7 +4594,7 @@
         <v>167</v>
       </c>
       <c r="B65" s="18" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>113</v>
@@ -4608,7 +4605,7 @@
         <v>168</v>
       </c>
       <c r="B66" s="18" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>91</v>
@@ -30855,8 +30852,8 @@
   </sheetPr>
   <dimension ref="A1:AMG36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V34" activeCellId="0" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -46261,7 +46258,7 @@
       <c r="AMF15" s="0"/>
       <c r="AMG15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="96.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="96.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="37" t="s">
         <v>888</v>
       </c>
@@ -46308,7 +46305,7 @@
         <v>43</v>
       </c>
       <c r="F17" s="39" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G17" s="39" t="s">
         <v>39</v>
@@ -46512,16 +46509,16 @@
         <v>914</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>186</v>
+        <v>906</v>
       </c>
       <c r="E24" s="39" t="s">
-        <v>186</v>
+        <v>906</v>
       </c>
       <c r="F24" s="39" t="s">
-        <v>186</v>
+        <v>914</v>
       </c>
       <c r="G24" s="39" t="s">
-        <v>186</v>
+        <v>914</v>
       </c>
       <c r="H24" s="39" t="s">
         <v>186</v>
@@ -46608,10 +46605,10 @@
         <v>923</v>
       </c>
       <c r="F27" s="39" t="s">
-        <v>914</v>
+        <v>923</v>
       </c>
       <c r="G27" s="39" t="s">
-        <v>914</v>
+        <v>923</v>
       </c>
       <c r="H27" s="39" t="s">
         <v>186</v>
@@ -46794,7 +46791,7 @@
         <v>929</v>
       </c>
       <c r="H33" s="39" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
       <c r="AMD33" s="0"/>
       <c r="AME33" s="0"/>
@@ -46809,19 +46806,19 @@
         <v>39</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="F34" s="39" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="G34" s="39" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="H34" s="39" t="s">
         <v>39</v>
@@ -46863,28 +46860,28 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="37" t="s">
+        <v>931</v>
+      </c>
+      <c r="B36" s="41" t="s">
         <v>932</v>
       </c>
-      <c r="B36" s="41" t="s">
-        <v>933</v>
-      </c>
       <c r="C36" s="41" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D36" s="41" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E36" s="41" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F36" s="41" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="G36" s="41" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="H36" s="41" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AMD36" s="0"/>
       <c r="AME36" s="0"/>

</xml_diff>